<commit_message>
modified:   .gitignore 	modified:   collection.py 	modified:   credit_score.py 	new file:   days_taken.py 	deleted:    interestCalc.xlsx 	new file:   od_interest.py 	deleted:    report-0.csv 	deleted:    report-1.csv 	new file:   reports.py 	new file:   sanity_check_ess.py 	new file:   sanity_check_nbnl.py 	new file:   sanity_check_ph.py
</commit_message>
<xml_diff>
--- a/functions.xlsx
+++ b/functions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NadunJayathunga\OneDrive - NBN Holdings\Financials\Other\Programmes\Dashboards\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F132DBB-56F8-415B-B2E4-27DBA424B418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F7220-1CBE-42B1-837C-A1A42F3D72A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{2BBD31FC-6384-45BA-8DCD-7BFB82444EAD}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2BBD31FC-6384-45BA-8DCD-7BFB82444EAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="od_int" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
     <author>Nadun Jayathunga</author>
   </authors>
   <commentList>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{E8F89141-65C9-49CC-87C5-18B3F0ED80E7}">
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{E8F89141-65C9-49CC-87C5-18B3F0ED80E7}">
       <text>
         <r>
           <rPr>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="64">
   <si>
     <t>tiv</t>
   </si>
@@ -121,9 +122,6 @@
     <t>Job Number</t>
   </si>
   <si>
-    <t>Service Description</t>
-  </si>
-  <si>
     <t>Sales Rate</t>
   </si>
   <si>
@@ -188,13 +186,91 @@
   </si>
   <si>
     <t>od_interest</t>
+  </si>
+  <si>
+    <t>Third Level Group Name</t>
+  </si>
+  <si>
+    <t>df_customers</t>
+  </si>
+  <si>
+    <t>Customer_Code</t>
+  </si>
+  <si>
+    <t>Cus_Name</t>
+  </si>
+  <si>
+    <t>Date_Established</t>
+  </si>
+  <si>
+    <t>Credit_Days</t>
+  </si>
+  <si>
+    <t>df_jobs</t>
+  </si>
+  <si>
+    <t>Job_Number</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>df_data(merged)</t>
+  </si>
+  <si>
+    <t>df_data_month</t>
+  </si>
+  <si>
+    <t>monthly_profit_report</t>
+  </si>
+  <si>
+    <t>Logistics Revenue - Clearance</t>
+  </si>
+  <si>
+    <t>Logistics Revenue - Freight</t>
+  </si>
+  <si>
+    <t>Logistics Revenue - Transport</t>
+  </si>
+  <si>
+    <t>Services Cost - Custom Clearance</t>
+  </si>
+  <si>
+    <t>Services Cost - Freight</t>
+  </si>
+  <si>
+    <t>Services Cost - Transport</t>
+  </si>
+  <si>
+    <t>s_c</t>
+  </si>
+  <si>
+    <t>s_t</t>
+  </si>
+  <si>
+    <t>s_f</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Cus_name</t>
+  </si>
+  <si>
+    <t>OD_Int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -239,8 +315,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +347,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -278,18 +366,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997F176E-6B27-4111-A87E-C4B654DB0CDD}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -641,14 +733,15 @@
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -675,11 +768,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -695,28 +788,24 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>20</v>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -742,117 +831,119 @@
       <c r="I5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>29</v>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10"/>
+      <c r="K8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f>C8</f>
         <v>Voucher_Date</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f>H8</f>
         <v>Voucher Number</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>30</v>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G11" t="s">
@@ -861,30 +952,31 @@
       <c r="H11" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
@@ -894,16 +986,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>34</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B14" t="str">
-        <f>K11</f>
+        <f>L11</f>
         <v>Credit</v>
       </c>
-      <c r="C14" s="10" t="str">
-        <f t="shared" ref="C14:D14" si="0">L11</f>
+      <c r="C14" s="9" t="str">
+        <f t="shared" ref="C14:D14" si="0">M11</f>
         <v>Voucher_Date</v>
       </c>
       <c r="D14" t="str">
@@ -911,107 +1003,107 @@
         <v>Voucher Number</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="10" t="str">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="9" t="str">
         <f>D11</f>
         <v>Ledger_Code</v>
       </c>
-      <c r="D16" s="10" t="str">
+      <c r="D16" s="9" t="str">
         <f>C11</f>
         <v>Voucher_Date</v>
       </c>
-      <c r="E16" s="10" t="str">
-        <f>J11</f>
+      <c r="E16" s="9" t="str">
+        <f>K11</f>
         <v>Net</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>19</v>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="C18" t="str">
-        <f>J5</f>
+        <f>K5</f>
         <v>Voucher Number</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>K5</f>
+        <f>L5</f>
         <v>Voucher_Date</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>L5</f>
+        <f>M5</f>
         <v>Credit</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>28</v>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="B20" t="str">
         <f>A5</f>
         <v>receipts_recorded</v>
       </c>
       <c r="C20" t="str">
-        <f>J5</f>
+        <f>K5</f>
         <v>Voucher Number</v>
       </c>
       <c r="D20" t="str">
-        <f>K5</f>
+        <f>L5</f>
         <v>Voucher_Date</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>L5</f>
+        <f>M5</f>
         <v>Credit</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>A8</f>
         <v>supplier_payments</v>
       </c>
       <c r="C21" t="str">
+        <f>M8</f>
+        <v>Voucher Number</v>
+      </c>
+      <c r="D21" t="str">
         <f>L8</f>
-        <v>Voucher Number</v>
-      </c>
-      <c r="D21" t="str">
-        <f>K8</f>
         <v>Voucher_Date</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="str">
+        <f>N11</f>
+        <v>Voucher Number</v>
+      </c>
+      <c r="D22" t="str">
+        <f>M11</f>
+        <v>Voucher_Date</v>
+      </c>
+      <c r="E22" t="str">
+        <f>L11</f>
+        <v>Credit</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C22" t="str">
-        <f>M11</f>
-        <v>Voucher Number</v>
-      </c>
-      <c r="D22" t="str">
-        <f>L11</f>
-        <v>Voucher_Date</v>
-      </c>
-      <c r="E22" t="str">
-        <f>K11</f>
-        <v>Credit</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="B24" t="str">
         <f>B11</f>
         <v>df_data</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E24" t="s">
@@ -1029,68 +1121,68 @@
       <c r="I24" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>22</v>
+      <c r="E25" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>B12</f>
         <v>coa</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" t="str">
         <f>A20</f>
@@ -1109,26 +1201,276 @@
         <v>Credit</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>A5</f>
         <v>receipts_recorded</v>
       </c>
       <c r="C31" t="str">
-        <f>J5</f>
+        <f>K5</f>
         <v>Voucher Number</v>
       </c>
       <c r="D31" t="str">
-        <f>K5</f>
+        <f>L5</f>
         <v>Voucher_Date</v>
       </c>
       <c r="E31" t="str">
-        <f>L5</f>
+        <f>M5</f>
         <v>Credit</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C341B409-79D8-404B-9B6E-B91BBB97C8BE}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>